<commit_message>
CHT update - 08 Jul 2024 14:20
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sengl\Desktop\eiwg_webpage\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC65157-717C-4FCA-ABCC-5184C78D636A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{17130F81-5BF8-42BD-9123-0B5FBBD68513}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="20715" windowHeight="13875"/>
   </bookViews>
   <sheets>
     <sheet name="Members" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -425,8 +419,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,7 +461,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -492,26 +486,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B341FAF4-A4BA-4C23-AFA4-37DEBCD9376A}" name="Tabelle1" displayName="Tabelle1" ref="A1:N67" totalsRowShown="0">
-  <autoFilter ref="A1:N67" xr:uid="{B341FAF4-A4BA-4C23-AFA4-37DEBCD9376A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:N67" totalsRowShown="0">
+  <autoFilter ref="A1:N67"/>
+  <sortState ref="A2:M63">
     <sortCondition ref="B1:B63"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{D08EB286-1975-4440-9BD9-194C9243149F}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{0255C489-D014-4274-8CB1-E4292220887D}" name="Company"/>
-    <tableColumn id="4" xr3:uid="{0F16DAA8-9C6C-4829-8042-E0E7228903F3}" name="Function"/>
-    <tableColumn id="5" xr3:uid="{286CCCF0-16E8-4E77-A9A3-A45B4911B2BB}" name="Lead" dataDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{681642AA-A349-4C63-935B-8DE7EC58D0D3}" name="Type"/>
-    <tableColumn id="6" xr3:uid="{C61B0CC2-BE8D-4C61-B157-DBFABE9B8156}" name="Contact to"/>
-    <tableColumn id="7" xr3:uid="{745E10A6-79E0-4F5A-97B5-B9615B334A62}" name="Training"/>
-    <tableColumn id="8" xr3:uid="{1713FCF7-7F16-4EE7-951B-135DBE834827}" name="Estimation"/>
-    <tableColumn id="9" xr3:uid="{A6C0453F-11FB-4ACC-AB43-FFC7D6E963B7}" name="Reporting"/>
-    <tableColumn id="10" xr3:uid="{F4B23871-8281-40EC-9A17-B958306997F5}" name="EarlyPhase"/>
-    <tableColumn id="14" xr3:uid="{702C6A9C-BDB9-4B75-9BCF-F61453B4174B}" name="LateStage"/>
-    <tableColumn id="11" xr3:uid="{454BFB0F-D387-4A8A-A3DE-B73C1135FC0F}" name="NonInferiority"/>
-    <tableColumn id="12" xr3:uid="{C9E328C9-1AB1-4E70-B567-39E431ECD5AF}" name="Communications"/>
-    <tableColumn id="15" xr3:uid="{FFECF483-F5B5-481F-89AD-788FD7D1B97C}" name="IntercurrentEvent"/>
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="3" name="Company"/>
+    <tableColumn id="4" name="Function"/>
+    <tableColumn id="5" name="Lead" dataDxfId="0"/>
+    <tableColumn id="13" name="Type"/>
+    <tableColumn id="6" name="Contact to"/>
+    <tableColumn id="7" name="Training"/>
+    <tableColumn id="8" name="Estimation"/>
+    <tableColumn id="9" name="Reporting"/>
+    <tableColumn id="10" name="EarlyPhase"/>
+    <tableColumn id="14" name="LateStage"/>
+    <tableColumn id="11" name="NonInferiority"/>
+    <tableColumn id="12" name="Communications"/>
+    <tableColumn id="15" name="IntercurrentEvent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -560,7 +554,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -612,7 +606,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -806,39 +800,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69F38D8-CC18-441C-83B7-ACFF18261279}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.73046875" customWidth="1"/>
+    <col min="2" max="2" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.53125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" customWidth="1"/>
-    <col min="10" max="11" width="13.1796875" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" customWidth="1"/>
+    <col min="6" max="6" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.53125" customWidth="1"/>
+    <col min="9" max="9" width="11.796875" customWidth="1"/>
+    <col min="10" max="11" width="13.19921875" customWidth="1"/>
+    <col min="12" max="12" width="16.796875" customWidth="1"/>
     <col min="13" max="14" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -882,7 +876,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -896,7 +890,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -919,7 +913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -948,7 +942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -971,7 +965,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -997,7 +991,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1014,7 +1008,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1028,7 +1022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1042,7 +1036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1065,7 +1059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1079,7 +1073,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1096,7 +1090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1110,7 +1104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1130,7 +1124,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1147,7 +1141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1176,7 +1170,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1190,7 +1184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1207,7 +1201,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1224,7 +1218,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1241,7 +1235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1255,7 +1249,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1272,7 +1266,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1286,7 +1280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1303,7 +1297,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1317,7 +1311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1343,7 +1337,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1360,7 +1354,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1377,7 +1371,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -1391,7 +1385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -1408,7 +1402,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -1422,7 +1416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1442,7 +1436,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -1456,7 +1450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -1473,7 +1467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -1487,7 +1481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -1513,7 +1507,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -1527,7 +1521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -1547,7 +1541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>85</v>
       </c>
@@ -1567,7 +1561,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -1599,7 +1593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>89</v>
       </c>
@@ -1616,7 +1610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -1633,7 +1627,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="15" customHeight="1">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -1650,7 +1644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>92</v>
       </c>
@@ -1667,7 +1661,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -1681,7 +1675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -1695,7 +1689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="15" customHeight="1">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -1718,7 +1712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" ht="15" customHeight="1">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -1735,7 +1729,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" ht="15" customHeight="1">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -1758,7 +1752,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -1775,7 +1769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -1792,7 +1786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -1809,7 +1803,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -1826,7 +1820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -1843,7 +1837,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -1860,7 +1854,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -1877,7 +1871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -1894,7 +1888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>110</v>
       </c>
@@ -1908,7 +1902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
         <v>112</v>
       </c>
@@ -1928,7 +1922,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
         <v>114</v>
       </c>
@@ -1942,7 +1936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
         <v>115</v>
       </c>
@@ -1965,7 +1959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
         <v>117</v>
       </c>
@@ -1979,7 +1973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -2005,7 +1999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14">
       <c r="A64" t="s">
         <v>119</v>
       </c>
@@ -2019,12 +2013,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14">
       <c r="A65" t="s">
         <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C65" t="s">
         <v>12</v>
@@ -2042,7 +2036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14">
       <c r="A66" t="s">
         <v>121</v>
       </c>
@@ -2059,7 +2053,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14">
       <c r="A67" t="s">
         <v>123</v>
       </c>
@@ -2075,15 +2069,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A60" r:id="rId1" display="mailto:Katsumi.Yoshida@ucb.com" xr:uid="{3C812578-DD1B-49BB-A242-5263405B1626}"/>
-    <hyperlink ref="A32" r:id="rId2" display="mailto:Armin.Schueler@merckgroup.com" xr:uid="{0C1B3D6B-7EB6-44A6-AFDA-04CAAF92CB60}"/>
-    <hyperlink ref="A47" r:id="rId3" display="mailto:Sue.McKendrick@ppdi.com" xr:uid="{515BE35B-5A85-48BC-BC16-BAD38381277F}"/>
-    <hyperlink ref="A58" r:id="rId4" display="mailto:estelle.lambert@servier.com" xr:uid="{6406BE5F-4FA6-4BA4-8B37-DFFD1761F32D}"/>
-    <hyperlink ref="A14" r:id="rId5" display="mailto:Lorenzo.Guizzaro@ema.europa.eu" xr:uid="{53C82E9C-134D-4456-B765-B8C1AC0BBD26}"/>
-    <hyperlink ref="A22" r:id="rId6" display="mailto:oliverkeene405@gmail.com" xr:uid="{3AEF5FB4-2147-49FA-9471-58EC544AD4C2}"/>
-    <hyperlink ref="A12" r:id="rId7" display="mailto:s.vezzoli@chiesi.com" xr:uid="{1DCE2109-1515-4931-B35F-F18BE5A84BD4}"/>
-    <hyperlink ref="A21" r:id="rId8" display="mailto:carrie.li@idorsia.com" xr:uid="{3B6A482F-1404-4152-85E5-A4AED8123625}"/>
-    <hyperlink ref="A65" r:id="rId9" display="mailto:chun-hang.x.tang@gsk.com" xr:uid="{53CA39C7-9313-4E5B-B071-0C95848570CE}"/>
+    <hyperlink ref="A60" r:id="rId1" display="mailto:Katsumi.Yoshida@ucb.com"/>
+    <hyperlink ref="A32" r:id="rId2" display="mailto:Armin.Schueler@merckgroup.com"/>
+    <hyperlink ref="A47" r:id="rId3" display="mailto:Sue.McKendrick@ppdi.com"/>
+    <hyperlink ref="A58" r:id="rId4" display="mailto:estelle.lambert@servier.com"/>
+    <hyperlink ref="A14" r:id="rId5" display="mailto:Lorenzo.Guizzaro@ema.europa.eu"/>
+    <hyperlink ref="A22" r:id="rId6" display="mailto:oliverkeene405@gmail.com"/>
+    <hyperlink ref="A12" r:id="rId7" display="mailto:s.vezzoli@chiesi.com"/>
+    <hyperlink ref="A21" r:id="rId8" display="mailto:carrie.li@idorsia.com"/>
+    <hyperlink ref="A65" r:id="rId9" display="mailto:chun-hang.x.tang@gsk.com"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="landscape" r:id="rId10"/>
@@ -2094,6 +2088,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C2547C8CC7B331428FF953FE0CD11F32" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c214334a35d04babb002cae86a5d4534">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fe6cebb0-ac24-4097-a45b-aec9fe749aaa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d936c9f92a69a3898e11e942e5a3cfa5" ns2:_="">
     <xsd:import namespace="fe6cebb0-ac24-4097-a45b-aec9fe749aaa"/>
@@ -2237,22 +2246,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1288C358-E90E-46A5-8B49-D40D5385BECC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5478ECA-E19E-4E78-97DE-7171B34BD30F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A80BF24A-4978-4F18-B8A8-A4B8F8FB685A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2268,21 +2279,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5478ECA-E19E-4E78-97DE-7171B34BD30F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1288C358-E90E-46A5-8B49-D40D5385BECC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Study Design Subteam Add Publication
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e85c81c27d35d093/Dokumente/Webseiten/EIWG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_1329E47AF590188FDA5ACF01FB3FC0173EAA5361" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07A0ECD3-F436-4112-BA2E-3CD1CADCB920}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_1329E47AF590188FDA5ACF01FB3FC0173EAA5361" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0903B50-8DFF-4770-9F6D-529E921A9E17}"/>
   <bookViews>
     <workbookView xWindow="6000" yWindow="2040" windowWidth="18000" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="170">
   <si>
     <t>Name</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Amel Besseghir</t>
   </si>
   <si>
-    <t>Fresenius</t>
-  </si>
-  <si>
     <t>Co-Lead EIWG</t>
   </si>
   <si>
@@ -254,9 +251,6 @@
     <t>Armin Schueler</t>
   </si>
   <si>
-    <t>Morphosys</t>
-  </si>
-  <si>
     <t>PhUSE</t>
   </si>
   <si>
@@ -534,6 +528,24 @@
   </si>
   <si>
     <t>Liyi Jia</t>
+  </si>
+  <si>
+    <t>StudyDesign</t>
+  </si>
+  <si>
+    <t>Fortrea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bharani Dharan </t>
+  </si>
+  <si>
+    <t>Jay Park</t>
+  </si>
+  <si>
+    <t>McMaster Univ, Canada</t>
+  </si>
+  <si>
+    <t>Simon Newsome</t>
   </si>
 </sst>
 </file>
@@ -585,11 +597,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -622,9 +635,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{374549D1-D3BF-4254-BDF5-218289279DEE}" name="Tabelle1" displayName="Tabelle1" ref="A1:O95" totalsRowShown="0">
-  <autoFilter ref="A1:O95" xr:uid="{374549D1-D3BF-4254-BDF5-218289279DEE}"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{374549D1-D3BF-4254-BDF5-218289279DEE}" name="Tabelle1" displayName="Tabelle1" ref="A1:P98" totalsRowShown="0">
+  <autoFilter ref="A1:P98" xr:uid="{374549D1-D3BF-4254-BDF5-218289279DEE}"/>
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{90DF7BE4-4C7E-4F3D-8B33-9661BC441C08}" name="Name"/>
     <tableColumn id="3" xr3:uid="{A1F942EC-54E9-41B8-8BB5-1C9D8F099D48}" name="Company"/>
     <tableColumn id="4" xr3:uid="{84EA482C-8A73-4DDA-9B80-62BFFDB3C597}" name="Function"/>
@@ -640,6 +653,7 @@
     <tableColumn id="12" xr3:uid="{20ABD840-DC0C-4E0B-A7B9-C98DE73BC326}" name="Communications"/>
     <tableColumn id="15" xr3:uid="{B6AE1A02-44B1-4692-B69D-F92D86AB0CC0}" name="IntercurrentEvent"/>
     <tableColumn id="2" xr3:uid="{E40105CC-553A-4713-9BF9-D2090938F157}" name="US"/>
+    <tableColumn id="16" xr3:uid="{D8EB0BF8-2E74-4901-B179-B0F7456ABA00}" name="StudyDesign"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -945,10 +959,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O95"/>
+  <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -966,7 +980,7 @@
     <col min="13" max="14" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1010,10 +1024,13 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+      <c r="P1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1027,7 +1044,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1047,61 +1064,64 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1119,63 +1139,63 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="L7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -1192,265 +1212,277 @@
       <c r="N10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B11" t="s">
-        <v>141</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>38</v>
       </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" t="s">
-        <v>20</v>
-      </c>
-      <c r="N16" t="s">
-        <v>20</v>
-      </c>
-      <c r="O16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
         <v>44</v>
       </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>45</v>
       </c>
-      <c r="E17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>47</v>
       </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>48</v>
       </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>49</v>
       </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>51</v>
       </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>53</v>
       </c>
-      <c r="C22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" t="s">
-        <v>17</v>
-      </c>
-      <c r="L22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="P23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>54</v>
       </c>
-      <c r="B23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>55</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="C24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>58</v>
       </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
       <c r="B26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
@@ -1462,103 +1494,103 @@
         <v>17</v>
       </c>
       <c r="F26" t="s">
+        <v>59</v>
+      </c>
+      <c r="M26" t="s">
+        <v>20</v>
+      </c>
+      <c r="N26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>60</v>
       </c>
-      <c r="M26" t="s">
-        <v>20</v>
-      </c>
-      <c r="N26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="B27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>62</v>
       </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>63</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>64</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>65</v>
       </c>
-      <c r="E28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>66</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>67</v>
       </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>68</v>
       </c>
-      <c r="B30" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>69</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
         <v>71</v>
-      </c>
-      <c r="B32" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" t="s">
-        <v>73</v>
       </c>
       <c r="N32" t="s">
         <v>20</v>
@@ -1566,10 +1598,10 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
         <v>16</v>
@@ -1580,16 +1612,16 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L34" t="s">
         <v>20</v>
@@ -1597,10 +1629,10 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
         <v>16</v>
@@ -1611,10 +1643,10 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s">
         <v>16</v>
@@ -1637,10 +1669,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C37" t="s">
         <v>16</v>
@@ -1651,10 +1683,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
@@ -1668,16 +1700,16 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H39" t="s">
         <v>20</v>
@@ -1688,10 +1720,10 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C40" t="s">
         <v>16</v>
@@ -1703,7 +1735,7 @@
         <v>17</v>
       </c>
       <c r="F40" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G40" t="s">
         <v>20</v>
@@ -1720,13 +1752,13 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E41" t="s">
         <v>17</v>
@@ -1734,10 +1766,10 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
         <v>16</v>
@@ -1751,16 +1783,16 @@
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
         <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J43" t="s">
         <v>20</v>
@@ -1768,27 +1800,27 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
         <v>16</v>
       </c>
       <c r="E44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E45" t="s">
         <v>17</v>
@@ -1796,13 +1828,13 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E46" t="s">
         <v>17</v>
@@ -1810,10 +1842,10 @@
     </row>
     <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
         <v>16</v>
@@ -1836,216 +1868,216 @@
     </row>
     <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
         <v>98</v>
       </c>
-      <c r="B48" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" t="s">
-        <v>47</v>
-      </c>
-      <c r="E48" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="C49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>99</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>100</v>
       </c>
-      <c r="C49" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" t="s">
-        <v>17</v>
-      </c>
-      <c r="G49" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>101</v>
       </c>
-      <c r="B50" t="s">
-        <v>100</v>
-      </c>
-      <c r="C50" t="s">
-        <v>47</v>
-      </c>
-      <c r="E50" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="B52" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>102</v>
       </c>
-      <c r="B51" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" t="s">
-        <v>16</v>
-      </c>
-      <c r="E51" t="s">
-        <v>29</v>
-      </c>
-      <c r="L51" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="B53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>103</v>
       </c>
-      <c r="B52" t="s">
-        <v>100</v>
-      </c>
-      <c r="C52" t="s">
-        <v>16</v>
-      </c>
-      <c r="E52" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+      <c r="B54" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" t="s">
+        <v>28</v>
+      </c>
+      <c r="L54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>104</v>
       </c>
-      <c r="B53" t="s">
-        <v>100</v>
-      </c>
-      <c r="C53" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" t="s">
-        <v>29</v>
-      </c>
-      <c r="H53" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+      <c r="B55" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>105</v>
       </c>
-      <c r="B54" t="s">
-        <v>100</v>
-      </c>
-      <c r="C54" t="s">
-        <v>16</v>
-      </c>
-      <c r="E54" t="s">
-        <v>29</v>
-      </c>
-      <c r="L54" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="B56" t="s">
         <v>106</v>
       </c>
-      <c r="B55" t="s">
-        <v>100</v>
-      </c>
-      <c r="C55" t="s">
-        <v>45</v>
-      </c>
-      <c r="E55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>107</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" t="s">
+        <v>28</v>
+      </c>
+      <c r="L57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>108</v>
       </c>
-      <c r="C56" t="s">
-        <v>16</v>
-      </c>
-      <c r="E56" t="s">
-        <v>29</v>
-      </c>
-      <c r="L56" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="B58" t="s">
         <v>109</v>
       </c>
-      <c r="B57" t="s">
-        <v>108</v>
-      </c>
-      <c r="C57" t="s">
-        <v>16</v>
-      </c>
-      <c r="E57" t="s">
-        <v>29</v>
-      </c>
-      <c r="L57" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>110</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>111</v>
       </c>
-      <c r="C58" t="s">
-        <v>16</v>
-      </c>
-      <c r="E58" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="C59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" t="s">
+        <v>17</v>
+      </c>
+      <c r="I59" t="s">
+        <v>20</v>
+      </c>
+      <c r="N59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>112</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>113</v>
       </c>
-      <c r="C59" t="s">
-        <v>16</v>
-      </c>
-      <c r="E59" t="s">
-        <v>17</v>
-      </c>
-      <c r="I59" t="s">
-        <v>20</v>
-      </c>
-      <c r="N59" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+      <c r="B61" t="s">
         <v>114</v>
-      </c>
-      <c r="B60" t="s">
-        <v>113</v>
-      </c>
-      <c r="C60" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>115</v>
-      </c>
-      <c r="B61" t="s">
-        <v>116</v>
       </c>
       <c r="C61" t="s">
         <v>16</v>
@@ -2063,26 +2095,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B62" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" t="s">
+        <v>17</v>
+      </c>
+      <c r="P62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>116</v>
       </c>
-      <c r="C62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>118</v>
-      </c>
       <c r="B63" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C63" t="s">
         <v>16</v>
@@ -2097,12 +2132,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C64" t="s">
         <v>16</v>
@@ -2114,9 +2149,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B65" t="s">
         <v>19</v>
@@ -2137,250 +2172,256 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" t="s">
+        <v>120</v>
+      </c>
+      <c r="C66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+      <c r="J66" t="s">
+        <v>20</v>
+      </c>
+      <c r="N66" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>121</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
+        <v>91</v>
+      </c>
+      <c r="C67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="G67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C66" t="s">
-        <v>16</v>
-      </c>
-      <c r="E66" t="s">
-        <v>17</v>
-      </c>
-      <c r="J66" t="s">
-        <v>20</v>
-      </c>
-      <c r="N66" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+      <c r="B68" t="s">
+        <v>39</v>
+      </c>
+      <c r="C68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" t="s">
+        <v>28</v>
+      </c>
+      <c r="N68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B67" t="s">
-        <v>93</v>
-      </c>
-      <c r="C67" t="s">
-        <v>16</v>
-      </c>
-      <c r="E67" t="s">
-        <v>17</v>
-      </c>
-      <c r="G67" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
+      <c r="B69" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" t="s">
+        <v>46</v>
+      </c>
+      <c r="E69" t="s">
+        <v>28</v>
+      </c>
+      <c r="J69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>124</v>
       </c>
-      <c r="B68" t="s">
-        <v>40</v>
-      </c>
-      <c r="C68" t="s">
-        <v>16</v>
-      </c>
-      <c r="E68" t="s">
-        <v>29</v>
-      </c>
-      <c r="N68" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A69" s="3" t="s">
+      <c r="B70" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" t="s">
+        <v>28</v>
+      </c>
+      <c r="J70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>125</v>
       </c>
-      <c r="B69" t="s">
-        <v>80</v>
-      </c>
-      <c r="C69" t="s">
-        <v>47</v>
-      </c>
-      <c r="E69" t="s">
-        <v>29</v>
-      </c>
-      <c r="J69" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+      <c r="B71" t="s">
+        <v>98</v>
+      </c>
+      <c r="C71" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>126</v>
       </c>
-      <c r="B70" t="s">
-        <v>96</v>
-      </c>
-      <c r="C70" t="s">
-        <v>16</v>
-      </c>
-      <c r="E70" t="s">
-        <v>29</v>
-      </c>
-      <c r="J70" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+      <c r="B72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" t="s">
         <v>127</v>
       </c>
-      <c r="B71" t="s">
-        <v>100</v>
-      </c>
-      <c r="C71" t="s">
-        <v>16</v>
-      </c>
-      <c r="E71" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+      <c r="E72" t="s">
+        <v>28</v>
+      </c>
+      <c r="I72" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>128</v>
       </c>
-      <c r="B72" t="s">
-        <v>27</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B73" t="s">
+        <v>42</v>
+      </c>
+      <c r="C73" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" t="s">
+        <v>28</v>
+      </c>
+      <c r="I73" t="s">
+        <v>20</v>
+      </c>
+      <c r="P73" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>129</v>
       </c>
-      <c r="E72" t="s">
-        <v>29</v>
-      </c>
-      <c r="I72" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+      <c r="B74" t="s">
+        <v>26</v>
+      </c>
+      <c r="C74" t="s">
+        <v>127</v>
+      </c>
+      <c r="E74" t="s">
+        <v>28</v>
+      </c>
+      <c r="I74" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>130</v>
       </c>
-      <c r="B73" t="s">
-        <v>43</v>
-      </c>
-      <c r="C73" t="s">
-        <v>16</v>
-      </c>
-      <c r="E73" t="s">
-        <v>29</v>
-      </c>
-      <c r="I73" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+      <c r="B75" t="s">
         <v>131</v>
       </c>
-      <c r="B74" t="s">
-        <v>27</v>
-      </c>
-      <c r="C74" t="s">
-        <v>129</v>
-      </c>
-      <c r="E74" t="s">
-        <v>29</v>
-      </c>
-      <c r="I74" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+      <c r="C75" t="s">
+        <v>140</v>
+      </c>
+      <c r="E75" t="s">
+        <v>28</v>
+      </c>
+      <c r="I75" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>132</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
+        <v>131</v>
+      </c>
+      <c r="C76" t="s">
+        <v>141</v>
+      </c>
+      <c r="E76" t="s">
+        <v>28</v>
+      </c>
+      <c r="I76" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>133</v>
       </c>
-      <c r="C75" t="s">
+      <c r="B77" t="s">
+        <v>131</v>
+      </c>
+      <c r="C77" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" t="s">
+        <v>28</v>
+      </c>
+      <c r="I77" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>134</v>
+      </c>
+      <c r="B78" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" t="s">
+        <v>17</v>
+      </c>
+      <c r="I78" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>137</v>
+      </c>
+      <c r="B79" t="s">
+        <v>138</v>
+      </c>
+      <c r="C79" t="s">
+        <v>16</v>
+      </c>
+      <c r="E79" t="s">
+        <v>28</v>
+      </c>
+      <c r="H79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>142</v>
       </c>
-      <c r="E75" t="s">
-        <v>29</v>
-      </c>
-      <c r="I75" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>134</v>
-      </c>
-      <c r="B76" t="s">
-        <v>133</v>
-      </c>
-      <c r="C76" t="s">
-        <v>143</v>
-      </c>
-      <c r="E76" t="s">
-        <v>29</v>
-      </c>
-      <c r="I76" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>135</v>
-      </c>
-      <c r="B77" t="s">
-        <v>133</v>
-      </c>
-      <c r="C77" t="s">
-        <v>16</v>
-      </c>
-      <c r="E77" t="s">
-        <v>29</v>
-      </c>
-      <c r="I77" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>136</v>
-      </c>
-      <c r="B78" t="s">
-        <v>84</v>
-      </c>
-      <c r="C78" t="s">
-        <v>16</v>
-      </c>
-      <c r="E78" t="s">
-        <v>17</v>
-      </c>
-      <c r="I78" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>139</v>
-      </c>
-      <c r="B79" t="s">
-        <v>140</v>
-      </c>
-      <c r="C79" t="s">
-        <v>16</v>
-      </c>
-      <c r="E79" t="s">
-        <v>29</v>
-      </c>
-      <c r="H79" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>144</v>
-      </c>
       <c r="B80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C80" t="s">
         <v>16</v>
@@ -2391,16 +2432,16 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B81" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C81" t="s">
         <v>16</v>
       </c>
       <c r="E81" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K81" t="s">
         <v>20</v>
@@ -2408,16 +2449,16 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B82" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C82" t="s">
         <v>16</v>
       </c>
       <c r="E82" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K82" t="s">
         <v>20</v>
@@ -2425,16 +2466,16 @@
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C83" t="s">
         <v>16</v>
       </c>
       <c r="E83" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K83" t="s">
         <v>20</v>
@@ -2442,16 +2483,16 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B84" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C84" t="s">
         <v>16</v>
       </c>
       <c r="E84" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K84" t="s">
         <v>20</v>
@@ -2459,16 +2500,16 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B85" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C85" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E85" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I85" t="s">
         <v>20</v>
@@ -2476,16 +2517,16 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B86" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C86" t="s">
         <v>16</v>
       </c>
       <c r="D86" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E86" t="s">
         <v>17</v>
@@ -2496,10 +2537,10 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B87" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C87" t="s">
         <v>16</v>
@@ -2513,16 +2554,16 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B88" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C88" t="s">
         <v>16</v>
       </c>
       <c r="D88" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E88" t="s">
         <v>17</v>
@@ -2533,7 +2574,7 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B89" t="s">
         <v>15</v>
@@ -2550,10 +2591,10 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B90" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C90" t="s">
         <v>16</v>
@@ -2567,10 +2608,10 @@
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B91" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C91" t="s">
         <v>16</v>
@@ -2584,10 +2625,10 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B92" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C92" t="s">
         <v>16</v>
@@ -2601,10 +2642,10 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B93" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C93" t="s">
         <v>16</v>
@@ -2618,10 +2659,10 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B94" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C94" t="s">
         <v>16</v>
@@ -2635,10 +2676,10 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B95" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C95" t="s">
         <v>16</v>
@@ -2647,20 +2688,72 @@
         <v>17</v>
       </c>
       <c r="O95" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>166</v>
+      </c>
+      <c r="B96" t="s">
+        <v>82</v>
+      </c>
+      <c r="C96" t="s">
+        <v>16</v>
+      </c>
+      <c r="E96" t="s">
+        <v>17</v>
+      </c>
+      <c r="O96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>167</v>
+      </c>
+      <c r="B97" t="s">
+        <v>168</v>
+      </c>
+      <c r="C97" t="s">
+        <v>16</v>
+      </c>
+      <c r="E97" t="s">
+        <v>17</v>
+      </c>
+      <c r="O97" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>169</v>
+      </c>
+      <c r="B98" t="s">
+        <v>82</v>
+      </c>
+      <c r="C98" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98" s="4"/>
+      <c r="E98" t="s">
+        <v>28</v>
+      </c>
+      <c r="P98" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A60" r:id="rId1" display="mailto:Katsumi.Yoshida@ucb.com" xr:uid="{EBE20478-0968-4A4C-9171-AFBA9AA25304}"/>
-    <hyperlink ref="A32" r:id="rId2" display="mailto:Armin.Schueler@merckgroup.com" xr:uid="{7FE4F43F-8A17-4F8F-B8CF-66589B4EC62D}"/>
-    <hyperlink ref="A47" r:id="rId3" display="mailto:Sue.McKendrick@ppdi.com" xr:uid="{FC8E08CC-F9FD-49C9-98F5-35841E7A191A}"/>
-    <hyperlink ref="A58" r:id="rId4" display="mailto:estelle.lambert@servier.com" xr:uid="{3E5F75DC-5AA3-4E26-9A70-397321E235E8}"/>
-    <hyperlink ref="A14" r:id="rId5" display="mailto:Lorenzo.Guizzaro@ema.europa.eu" xr:uid="{B609E4ED-43F2-449D-B514-A11A9D6CDB7E}"/>
-    <hyperlink ref="A22" r:id="rId6" display="mailto:oliverkeene405@gmail.com" xr:uid="{619E57BA-8A59-442D-B97B-532671E67D5C}"/>
-    <hyperlink ref="A12" r:id="rId7" display="mailto:s.vezzoli@chiesi.com" xr:uid="{50C23274-35E9-426D-AD86-7FC7D8128987}"/>
-    <hyperlink ref="A21" r:id="rId8" display="mailto:carrie.li@idorsia.com" xr:uid="{AEED1870-BD95-46F7-90DE-3C8C4664F215}"/>
-    <hyperlink ref="A65" r:id="rId9" display="mailto:chun-hang.x.tang@gsk.com" xr:uid="{DE9D1F4C-140D-4B19-964E-938B9E178C22}"/>
+    <hyperlink ref="A60" r:id="rId1" display="mailto:Katsumi.Yoshida@ucb.com" xr:uid="{C44700A6-7F76-434C-8DD3-7FA23A81C240}"/>
+    <hyperlink ref="A32" r:id="rId2" display="mailto:Armin.Schueler@merckgroup.com" xr:uid="{E3EB23F8-0296-4745-B451-F3E2620CDFA2}"/>
+    <hyperlink ref="A47" r:id="rId3" display="mailto:Sue.McKendrick@ppdi.com" xr:uid="{2606AD7B-CA23-4311-99BC-56B64B4C1464}"/>
+    <hyperlink ref="A58" r:id="rId4" display="mailto:estelle.lambert@servier.com" xr:uid="{8E83AE87-7E63-4540-A7B4-78CF7CEA3126}"/>
+    <hyperlink ref="A14" r:id="rId5" display="mailto:Lorenzo.Guizzaro@ema.europa.eu" xr:uid="{ACB4D1D6-EF6C-4A8E-BFFB-BC57D6BE6709}"/>
+    <hyperlink ref="A22" r:id="rId6" display="mailto:oliverkeene405@gmail.com" xr:uid="{8D6AA4DF-58D1-4282-9373-4162BB66C72F}"/>
+    <hyperlink ref="A12" r:id="rId7" display="mailto:s.vezzoli@chiesi.com" xr:uid="{E8448F41-9D86-4436-94EF-CE8F8F502017}"/>
+    <hyperlink ref="A21" r:id="rId8" display="mailto:carrie.li@idorsia.com" xr:uid="{90787F68-954D-4ED3-A503-1A21D5705858}"/>
+    <hyperlink ref="A65" r:id="rId9" display="mailto:chun-hang.x.tang@gsk.com" xr:uid="{B6279BC3-07BA-4E46-AD20-B16FBA109BC7}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="landscape" r:id="rId10"/>
@@ -2680,12 +2773,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100C2547C8CC7B331428FF953FE0CD11F32" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="21585f8105577c55a14177137b0f487c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fe6cebb0-ac24-4097-a45b-aec9fe749aaa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a739419b1432b2a493df12220e235f53" ns2:_="">
     <xsd:import namespace="fe6cebb0-ac24-4097-a45b-aec9fe749aaa"/>
@@ -2829,6 +2916,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1288C358-E90E-46A5-8B49-D40D5385BECC}">
   <ds:schemaRefs>
@@ -2838,15 +2931,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5478ECA-E19E-4E78-97DE-7171B34BD30F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E44DC42-D40D-4161-B416-680814B33C76}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2862,4 +2946,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5478ECA-E19E-4E78-97DE-7171B34BD30F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>